<commit_message>
Added angles for 4
</commit_message>
<xml_diff>
--- a/MeasuredAngles.xlsx
+++ b/MeasuredAngles.xlsx
@@ -1,23 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10410"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="28209"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/martinraming/Documents/MatLab/PMAA_Fracture/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Mar_ten/Documents/PMAA_Fracture/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6F77EB60-530A-A749-862D-815A1B1EEF2A}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3240" yWindow="520" windowWidth="25440" windowHeight="14520" xr2:uid="{AC23CD0A-EEAB-E949-A29B-C0FEBB2ABCE9}"/>
+    <workbookView xWindow="21920" yWindow="10860" windowWidth="25440" windowHeight="14520"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -45,7 +50,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -393,11 +398,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D05F8D00-9E9C-7B4D-831E-3F561230D99F}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J5" sqref="J5"/>
+      <selection activeCell="E4" sqref="E4:E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -477,6 +482,19 @@
       <c r="A5">
         <v>4</v>
       </c>
+      <c r="B5">
+        <v>17.515000000000001</v>
+      </c>
+      <c r="C5">
+        <v>17.707000000000001</v>
+      </c>
+      <c r="D5">
+        <v>21.404</v>
+      </c>
+      <c r="E5">
+        <f t="shared" si="0"/>
+        <v>19.555500000000002</v>
+      </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6">

</xml_diff>